<commit_message>
Changes to 3x3 GridMaze hardware:
- Rather than seperate tall and short variants there is now a single intermediate height version of the maze.

- IR illumination is now provided by IR module PCBs which connect to the maze hub board using a Molex Micro-Fit cable and can be daisy chained.

- Reduced Poke IR beam current from 50mA to 40mA.
</commit_message>
<xml_diff>
--- a/GridMaze/PCBs/maze_hub_1_1/maze_hub_1_1_BOM.xlsx
+++ b/GridMaze/PCBs/maze_hub_1_1/maze_hub_1_1_BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Hardware development\Maze hardware\PCBs\maze_hub_1_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Dropbox\Hardware development\pyControl\hardware\GridMaze\PCBs\maze_hub_1_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E5E8DEF-6D1B-428C-A5C5-606CB8618913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1770" windowWidth="16710" windowHeight="13680"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="116">
   <si>
     <t>Part</t>
   </si>
@@ -363,12 +364,21 @@
   </si>
   <si>
     <t>100K</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>Micro-Fit connector</t>
+  </si>
+  <si>
+    <t>43045-0210</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -712,11 +722,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,7 +924,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>113</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -923,47 +936,47 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="G9" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="H9">
-        <v>1668368</v>
+        <v>3103032</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="H10">
-        <v>176434</v>
+        <v>1668368</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -975,41 +988,38 @@
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H11">
-        <v>1960971</v>
+        <v>176434</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12">
-        <v>1206</v>
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1759446</v>
+        <v>19</v>
+      </c>
+      <c r="H12">
+        <v>1960971</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
@@ -1035,33 +1045,33 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>45</v>
+      <c r="D14">
+        <v>1206</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
         <v>23</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="4">
-        <v>1759265</v>
+        <v>24</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1759446</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
@@ -1087,33 +1097,33 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
         <v>23</v>
       </c>
       <c r="G16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16">
-        <v>2447623</v>
+        <v>47</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1759265</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
         <v>51</v>
@@ -1139,7 +1149,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
         <v>51</v>
@@ -1165,7 +1175,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>
@@ -1191,7 +1201,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
         <v>51</v>
@@ -1217,10 +1227,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -1235,18 +1245,18 @@
         <v>23</v>
       </c>
       <c r="G21" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H21">
-        <v>2447603</v>
+        <v>2447623</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -1261,18 +1271,18 @@
         <v>23</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H22">
-        <v>2447553</v>
+        <v>2447603</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -1287,87 +1297,90 @@
         <v>23</v>
       </c>
       <c r="G23" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="H23">
-        <v>2447634</v>
+        <v>2447553</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24">
-        <v>7805</v>
-      </c>
-      <c r="D24" t="s">
-        <v>27</v>
+        <v>107</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G24" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="H24">
-        <v>1652297</v>
+        <v>2447634</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>7805</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="F25" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="G25" t="s">
-        <v>105</v>
-      </c>
-      <c r="H25" t="s">
-        <v>9</v>
+        <v>30</v>
+      </c>
+      <c r="H25">
+        <v>1652297</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" t="s">
-        <v>80</v>
+        <v>74</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F26" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G26" t="s">
-        <v>79</v>
-      </c>
-      <c r="H26">
-        <v>2775977</v>
+        <v>105</v>
+      </c>
+      <c r="H26" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
         <v>79</v>
@@ -1390,77 +1403,77 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="F28" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="G28" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="H28">
-        <v>1840676</v>
+        <v>2775977</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>112</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="D29" t="s">
+        <v>63</v>
       </c>
       <c r="E29" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F29" t="s">
         <v>65</v>
       </c>
       <c r="G29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H29">
-        <v>4974992</v>
+        <v>1840676</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>72</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" t="s">
-        <v>9</v>
+        <v>66</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="F30" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="G30" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="H30">
-        <v>2751448</v>
+        <v>4974992</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1474,21 +1487,21 @@
         <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="F31" t="s">
         <v>89</v>
       </c>
       <c r="G31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H31">
-        <v>3051093</v>
+        <v>2751448</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -1511,7 +1524,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -1520,21 +1533,21 @@
         <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="F33" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="G33" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H33">
-        <v>7991916</v>
+        <v>3051093</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
@@ -1543,21 +1556,21 @@
         <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F34" t="s">
         <v>98</v>
       </c>
       <c r="G34" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H34">
-        <v>3225932</v>
+        <v>7991916</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
@@ -1580,50 +1593,70 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" t="s">
+        <v>99</v>
+      </c>
+      <c r="H36">
+        <v>3225932</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>101</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>102</v>
       </c>
-      <c r="D36" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s">
         <v>102</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G37" t="s">
         <v>104</v>
       </c>
-      <c r="H36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F37" s="2"/>
+      <c r="H37" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>91</v>
-      </c>
+      <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F46" s="2"/>
-    </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H47" s="1"/>
+      <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H48" s="1"/>
@@ -1631,9 +1664,12 @@
     <row r="49" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H49" s="1"/>
     </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H50" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F36" r:id="rId1"/>
+    <hyperlink ref="F37" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>